<commit_message>
fixes to starting soldiers
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D0D94D-7E7A-4A72-AEE4-3F09ADEB49ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F7BE5F-4353-416A-B1B1-FB6C8871AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">abilities!$A$10:$FS$312</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">characters!$A$3:$KX$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">characters!$A$3:$KZ$155</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7085" uniqueCount="2986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7105" uniqueCount="2986">
   <si>
     <t>Rank</t>
   </si>
@@ -9769,13 +9769,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:KX174"/>
+  <dimension ref="A1:KZ174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="JV4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="JT4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="KB4" sqref="KB4"/>
+      <selection pane="bottomRight" activeCell="JU8" sqref="JU8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9809,14 +9809,14 @@
     <col min="277" max="277" width="13.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="278" max="278" width="14.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="279" max="279" width="5.28515625" style="61" bestFit="1" customWidth="1"/>
-    <col min="280" max="292" width="9.140625" style="6"/>
-    <col min="293" max="293" width="5.28515625" style="61" bestFit="1" customWidth="1"/>
-    <col min="294" max="308" width="9.140625" style="6"/>
-    <col min="309" max="309" width="5.28515625" style="61" bestFit="1" customWidth="1"/>
-    <col min="310" max="16384" width="9.140625" style="6"/>
+    <col min="280" max="293" width="9.140625" style="6"/>
+    <col min="294" max="294" width="5.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="295" max="310" width="9.140625" style="6"/>
+    <col min="311" max="311" width="5.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="312" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:310" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:312" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>120</v>
       </c>
@@ -10008,25 +10008,25 @@
       <c r="JT1" s="20" t="s">
         <v>1659</v>
       </c>
-      <c r="KG1" s="60"/>
-      <c r="KH1" s="19" t="s">
+      <c r="KH1" s="60"/>
+      <c r="KI1" s="19" t="s">
         <v>1660</v>
       </c>
-      <c r="KW1" s="60"/>
-      <c r="KX1" s="19" t="s">
+      <c r="KY1" s="60"/>
+      <c r="KZ1" s="19" t="s">
         <v>2490</v>
       </c>
     </row>
-    <row r="2" spans="1:310" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:312" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="19"/>
       <c r="E2" s="47"/>
       <c r="F2" s="47"/>
       <c r="JI2" s="61"/>
       <c r="JS2" s="61"/>
-      <c r="KG2" s="61"/>
-      <c r="KW2" s="61"/>
-    </row>
-    <row r="3" spans="1:310" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KH2" s="61"/>
+      <c r="KY2" s="61"/>
+    </row>
+    <row r="3" spans="1:312" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>121</v>
       </c>
@@ -10901,64 +10901,70 @@
         <v>1683</v>
       </c>
       <c r="KF3" s="21" t="s">
+        <v>2571</v>
+      </c>
+      <c r="KG3" s="21" t="s">
         <v>2570</v>
       </c>
-      <c r="KG3" s="61" t="s">
+      <c r="KH3" s="61" t="s">
         <v>1535</v>
       </c>
-      <c r="KH3" s="21" t="s">
+      <c r="KI3" s="21" t="s">
         <v>1654</v>
       </c>
-      <c r="KI3" s="21" t="s">
+      <c r="KJ3" s="21" t="s">
         <v>1381</v>
       </c>
-      <c r="KJ3" s="21" t="s">
+      <c r="KK3" s="21" t="s">
         <v>1379</v>
       </c>
-      <c r="KK3" s="21" t="s">
+      <c r="KL3" s="21" t="s">
         <v>1505</v>
       </c>
-      <c r="KL3" s="21" t="s">
+      <c r="KM3" s="21" t="s">
         <v>1500</v>
       </c>
-      <c r="KM3" s="21" t="s">
+      <c r="KN3" s="21" t="s">
         <v>1383</v>
       </c>
-      <c r="KN3" s="21" t="s">
+      <c r="KO3" s="21" t="s">
         <v>1503</v>
       </c>
-      <c r="KO3" s="21" t="s">
+      <c r="KP3" s="21" t="s">
         <v>1606</v>
       </c>
-      <c r="KP3" s="21" t="s">
+      <c r="KQ3" s="21" t="s">
         <v>1386</v>
       </c>
-      <c r="KQ3" s="21" t="s">
+      <c r="KR3" s="21" t="s">
         <v>1387</v>
       </c>
-      <c r="KR3" s="21" t="s">
+      <c r="KS3" s="21" t="s">
         <v>1385</v>
       </c>
-      <c r="KS3" s="21" t="s">
+      <c r="KT3" s="21" t="s">
         <v>1602</v>
       </c>
-      <c r="KT3" s="21" t="s">
+      <c r="KU3" s="21" t="s">
         <v>1653</v>
       </c>
-      <c r="KU3" s="21" t="s">
+      <c r="KV3" s="21" t="s">
+        <v>2572</v>
+      </c>
+      <c r="KW3" s="21" t="s">
         <v>1509</v>
       </c>
-      <c r="KV3" s="21" t="s">
+      <c r="KX3" s="21" t="s">
         <v>1683</v>
       </c>
-      <c r="KW3" s="61" t="s">
+      <c r="KY3" s="61" t="s">
         <v>1535</v>
       </c>
-      <c r="KX3" s="22" t="s">
+      <c r="KZ3" s="22" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -11378,26 +11384,26 @@
       <c r="JZ4" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KL4" s="6" t="s">
+      <c r="KM4" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KP4" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KQ4" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KR4" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU4" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX4" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="5" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KS4" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW4" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ4" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="5" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -11810,22 +11816,22 @@
         <v>384</v>
       </c>
       <c r="JZ5" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KC5" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ5" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU5" s="6" t="s">
+      <c r="KP5" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX5" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="6" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KR5" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW5" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ5" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -12233,20 +12239,20 @@
       <c r="JX6" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP6" s="6" t="s">
+      <c r="KQ6" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ6" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU6" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX6" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KR6" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW6" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ6" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>94</v>
       </c>
@@ -12657,20 +12663,20 @@
       <c r="JW7" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KJ7" s="6" t="s">
+      <c r="KK7" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ7" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU7" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX7" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="8" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KR7" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW7" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ7" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
@@ -13054,17 +13060,17 @@
       <c r="JT8" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ8" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU8" s="6" t="s">
+      <c r="KR8" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW8" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX8" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="9" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KZ8" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
@@ -13468,17 +13474,17 @@
       <c r="JT9" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ9" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU9" s="6" t="s">
+      <c r="KR9" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW9" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX9" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ9" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>95</v>
       </c>
@@ -13885,17 +13891,17 @@
       <c r="JV10" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ10" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU10" s="6" t="s">
+      <c r="KR10" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW10" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX10" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ10" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>96</v>
       </c>
@@ -14293,17 +14299,17 @@
       <c r="KD11" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ11" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU11" s="6" t="s">
+      <c r="KR11" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW11" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX11" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="12" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ11" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
@@ -14689,20 +14695,20 @@
       <c r="JT12" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KF12" s="6" t="s">
+      <c r="KG12" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ12" s="6" t="s">
+      <c r="KR12" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU12" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX12" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW12" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ12" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>97</v>
       </c>
@@ -15105,20 +15111,20 @@
       <c r="KA13" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KJ13" s="6" t="s">
+      <c r="KK13" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ13" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU13" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX13" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="14" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KR13" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW13" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ13" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -15524,17 +15530,17 @@
       <c r="JZ14" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ14" s="6" t="s">
+      <c r="KR14" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU14" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX14" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="15" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW14" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ14" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="15" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
@@ -15945,20 +15951,20 @@
       <c r="KA15" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ15" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KT15" s="6" t="s">
+      <c r="KR15" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KU15" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU15" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX15" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="16" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW15" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ15" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
@@ -16347,23 +16353,23 @@
       <c r="JZ16" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ16" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KR16" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KT16" s="6" t="s">
+      <c r="KS16" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KU16" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU16" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX16" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="17" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW16" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ16" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
@@ -16769,20 +16775,20 @@
       <c r="KA17" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP17" s="6" t="s">
+      <c r="KQ17" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ17" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU17" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX17" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="18" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KR17" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW17" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ17" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
@@ -17175,17 +17181,17 @@
       <c r="JZ18" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ18" s="6" t="s">
+      <c r="KR18" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU18" s="6" t="s">
+      <c r="KW18" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX18" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="19" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ18" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="19" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>98</v>
       </c>
@@ -17581,20 +17587,20 @@
       <c r="KD19" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KK19" s="6" t="s">
+      <c r="KL19" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ19" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU19" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX19" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="20" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KR19" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW19" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ19" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
@@ -17976,26 +17982,26 @@
       <c r="KE20" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KL20" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KP20" s="6" t="s">
+      <c r="KM20" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KQ20" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KR20" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS20" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU20" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KV20" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW20" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KX20" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="21" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
@@ -18399,17 +18405,17 @@
       <c r="KA21" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ21" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU21" s="6" t="s">
+      <c r="KR21" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW21" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX21" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="22" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ21" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>99</v>
       </c>
@@ -18815,20 +18821,20 @@
       <c r="KD22" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KO22" s="6" t="s">
+      <c r="KP22" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ22" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU22" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX22" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="23" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KR22" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW22" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ22" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="23" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>100</v>
       </c>
@@ -19225,17 +19231,17 @@
       <c r="JZ23" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ23" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU23" s="6" t="s">
+      <c r="KR23" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW23" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX23" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="24" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KZ23" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
@@ -19643,17 +19649,17 @@
       <c r="JZ24" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ24" s="6" t="s">
+      <c r="KR24" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU24" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX24" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="25" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW24" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ24" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="25" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
@@ -20060,20 +20066,20 @@
       <c r="JZ25" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KN25" s="6" t="s">
+      <c r="KO25" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ25" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU25" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX25" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="26" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KR25" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW25" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ25" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>101</v>
       </c>
@@ -20470,23 +20476,23 @@
       <c r="JZ26" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KI26" s="6" t="s">
+      <c r="KJ26" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KO26" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KQ26" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU26" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX26" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="27" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KP26" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR26" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW26" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ26" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="27" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
@@ -20874,26 +20880,29 @@
       <c r="JT27" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JV27" s="6" t="s">
+      <c r="JZ27" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KF27" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="JZ27" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KK27" s="6" t="s">
+      <c r="KL27" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR27" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KV27" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ27" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU27" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX27" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="28" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW27" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ27" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="28" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
@@ -21283,13 +21292,10 @@
       <c r="JZ28" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK28" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KM28" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KO28" s="6" t="s">
+      <c r="KL28" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KN28" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KP28" s="6" t="s">
@@ -21298,20 +21304,23 @@
       <c r="KQ28" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KS28" s="6" t="s">
+      <c r="KR28" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KT28" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KT28" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KU28" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX28" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="29" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW28" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ28" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="29" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>102</v>
       </c>
@@ -21706,23 +21715,23 @@
       <c r="JZ29" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KN29" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KP29" s="6" t="s">
+      <c r="KO29" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KQ29" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ29" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU29" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX29" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="30" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KR29" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW29" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ29" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>28</v>
       </c>
@@ -22122,20 +22131,20 @@
       <c r="KA30" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ30" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KR30" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS30" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU30" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX30" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="31" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW30" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ30" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>29</v>
       </c>
@@ -22523,17 +22532,17 @@
       <c r="JZ31" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ31" s="6" t="s">
+      <c r="KR31" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU31" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX31" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="32" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW31" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ31" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -22902,17 +22911,17 @@
       <c r="JZ32" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ32" s="6" t="s">
+      <c r="KR32" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU32" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX32" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="33" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW32" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ32" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="33" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>31</v>
       </c>
@@ -23306,14 +23315,14 @@
       <c r="JZ33" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU33" s="6" t="s">
+      <c r="KW33" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX33" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="34" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ33" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="34" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -23727,20 +23736,20 @@
       <c r="JZ34" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KF34" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KQ34" s="6" t="s">
+      <c r="KG34" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR34" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU34" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX34" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="35" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW34" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ34" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="35" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
@@ -24131,20 +24140,20 @@
       <c r="JZ35" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK35" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KM35" s="6" t="s">
+      <c r="KL35" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KN35" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU35" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX35" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="36" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW35" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ35" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="36" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>34</v>
       </c>
@@ -24531,28 +24540,34 @@
         <v>384</v>
       </c>
       <c r="JW36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="JZ36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KF36" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="JZ36" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KL36" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KO36" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KR36" s="6" t="s">
+      <c r="KM36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KP36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KV36" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU36" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX36" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="37" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW36" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ36" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="37" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>35</v>
       </c>
@@ -24930,17 +24945,17 @@
       <c r="JZ37" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK37" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU37" s="6" t="s">
+      <c r="KL37" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW37" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX37" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="38" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KZ37" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="38" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>36</v>
       </c>
@@ -25327,17 +25342,17 @@
       <c r="JZ38" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KJ38" s="6" t="s">
+      <c r="KK38" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU38" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX38" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="39" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW38" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ38" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="39" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>37</v>
       </c>
@@ -25712,17 +25727,17 @@
       <c r="JZ39" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KT39" s="6" t="s">
+      <c r="KU39" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU39" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX39" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="40" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW39" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ39" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="40" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>103</v>
       </c>
@@ -26114,14 +26129,14 @@
       <c r="JZ40" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU40" s="6" t="s">
+      <c r="KW40" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX40" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="41" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ40" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="41" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>39</v>
       </c>
@@ -26500,14 +26515,14 @@
       <c r="JZ41" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU41" s="6" t="s">
+      <c r="KW41" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX41" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="42" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ41" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="42" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>40</v>
       </c>
@@ -26911,17 +26926,17 @@
       <c r="JZ42" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ42" s="6" t="s">
+      <c r="KR42" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU42" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX42" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="43" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW42" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ42" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="43" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>41</v>
       </c>
@@ -27302,17 +27317,17 @@
       <c r="JZ43" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK43" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU43" s="6" t="s">
+      <c r="KL43" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW43" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX43" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="44" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ43" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="44" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>42</v>
       </c>
@@ -27692,17 +27707,17 @@
       <c r="JZ44" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KS44" s="6" t="s">
+      <c r="KT44" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU44" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX44" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="45" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW44" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ44" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>104</v>
       </c>
@@ -28095,23 +28110,23 @@
       <c r="JZ45" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KM45" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KP45" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KT45" s="6" t="s">
+      <c r="KN45" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KQ45" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KU45" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU45" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX45" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="46" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW45" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ45" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="46" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>105</v>
       </c>
@@ -28524,19 +28539,16 @@
       <c r="JZ46" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KF46" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KK46" s="6" t="s">
+      <c r="KG46" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KL46" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KN46" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KP46" s="6" t="s">
+      <c r="KM46" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KO46" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KQ46" s="6" t="s">
@@ -28545,17 +28557,20 @@
       <c r="KR46" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU46" s="6" t="s">
+      <c r="KS46" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW46" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KV46" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KX46" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="47" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KZ46" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="47" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>106</v>
       </c>
@@ -28953,20 +28968,20 @@
       <c r="KB47" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KH47" s="6" t="s">
+      <c r="KI47" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KJ47" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KQ47" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU47" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="48" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KK47" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR47" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW47" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="48" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>46</v>
       </c>
@@ -29360,29 +29375,29 @@
       <c r="JZ48" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KH48" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KK48" s="6" t="s">
+      <c r="KI48" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KL48" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KM48" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KO48" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KQ48" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU48" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX48" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="49" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KP48" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR48" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW48" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ48" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="49" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>47</v>
       </c>
@@ -29802,20 +29817,20 @@
       <c r="JZ49" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KL49" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KR49" s="6" t="s">
+      <c r="KM49" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS49" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU49" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX49" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="50" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW49" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ49" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="50" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>107</v>
       </c>
@@ -30188,23 +30203,23 @@
       <c r="JZ50" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK50" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KN50" s="6" t="s">
+      <c r="KL50" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KO50" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ50" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU50" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX50" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="51" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KR50" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW50" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ50" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>108</v>
       </c>
@@ -30596,20 +30611,20 @@
       <c r="JZ51" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KS51" s="6" t="s">
+      <c r="KT51" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KT51" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KU51" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX51" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="52" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW51" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ51" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="52" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>109</v>
       </c>
@@ -31008,17 +31023,17 @@
       <c r="JZ52" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KL52" s="6" t="s">
+      <c r="KM52" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU52" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX52" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="53" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW52" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ52" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="53" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>51</v>
       </c>
@@ -31369,14 +31384,14 @@
       <c r="JZ53" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU53" s="6" t="s">
+      <c r="KW53" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX53" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="54" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ53" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="54" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -31772,17 +31787,17 @@
       <c r="JZ54" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ54" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU54" s="6" t="s">
+      <c r="KR54" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW54" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX54" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="55" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ54" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="55" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>110</v>
       </c>
@@ -32167,17 +32182,17 @@
       <c r="JZ55" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP55" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU55" s="6" t="s">
+      <c r="KQ55" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW55" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX55" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="56" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ55" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="56" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>54</v>
       </c>
@@ -32559,20 +32574,20 @@
       <c r="KE56" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KL56" s="6" t="s">
+      <c r="KM56" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KR56" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU56" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KV56" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="57" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KS56" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW56" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KX56" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>111</v>
       </c>
@@ -32956,17 +32971,17 @@
       <c r="KA57" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KL57" s="6" t="s">
+      <c r="KM57" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU57" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX57" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="58" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW57" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ57" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>56</v>
       </c>
@@ -33381,17 +33396,17 @@
       <c r="JZ58" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KL58" s="6" t="s">
+      <c r="KM58" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU58" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX58" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="59" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW58" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ58" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>112</v>
       </c>
@@ -33781,17 +33796,17 @@
       <c r="JZ59" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP59" s="6" t="s">
+      <c r="KQ59" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU59" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX59" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="60" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KW59" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ59" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>113</v>
       </c>
@@ -34223,26 +34238,26 @@
       <c r="KA60" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KK60" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KL60" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KM60" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KP60" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KT60" s="6" t="s">
+      <c r="KQ60" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KU60" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX60" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="61" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW60" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ60" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="61" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>114</v>
       </c>
@@ -34624,26 +34639,26 @@
       <c r="JZ61" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK61" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KN61" s="6" t="s">
+      <c r="KL61" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KO61" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ61" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU61" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KV61" s="6" t="s">
+      <c r="KR61" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW61" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KX61" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="62" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ61" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="62" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>60</v>
       </c>
@@ -35023,17 +35038,17 @@
       <c r="JZ62" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP62" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU62" s="6" t="s">
+      <c r="KQ62" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW62" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX62" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="63" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KZ62" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="63" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>61</v>
       </c>
@@ -35420,20 +35435,20 @@
       <c r="JZ63" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KN63" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KR63" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU63" s="6" t="s">
+      <c r="KO63" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS63" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW63" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX63" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="64" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ63" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>62</v>
       </c>
@@ -35810,14 +35825,14 @@
       <c r="JZ64" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU64" s="6" t="s">
+      <c r="KW64" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX64" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="65" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ64" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="65" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>63</v>
       </c>
@@ -36203,17 +36218,17 @@
       <c r="JZ65" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ65" s="6" t="s">
+      <c r="KR65" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU65" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX65" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="66" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW65" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ65" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="66" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>115</v>
       </c>
@@ -36596,17 +36611,17 @@
       <c r="JZ66" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KT66" s="6" t="s">
+      <c r="KU66" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU66" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX66" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="67" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW66" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ66" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="67" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>65</v>
       </c>
@@ -36998,17 +37013,17 @@
       <c r="KB67" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KH67" s="6" t="s">
+      <c r="KI67" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU67" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX67" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="68" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW67" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ67" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="68" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>66</v>
       </c>
@@ -37377,17 +37392,17 @@
       <c r="JZ68" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KR68" s="6" t="s">
+      <c r="KS68" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU68" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX68" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="69" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW68" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ68" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="69" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>67</v>
       </c>
@@ -37778,17 +37793,17 @@
       <c r="JZ69" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ69" s="6" t="s">
+      <c r="KR69" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU69" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX69" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="70" spans="1:310" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="KW69" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ69" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="70" spans="1:312" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>116</v>
       </c>
@@ -38174,17 +38189,17 @@
       <c r="KA70" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KR70" s="6" t="s">
+      <c r="KS70" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU70" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX70" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="71" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW70" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ70" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="71" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>117</v>
       </c>
@@ -38578,17 +38593,17 @@
       <c r="JZ71" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KP71" s="6" t="s">
+      <c r="KQ71" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU71" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX71" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="72" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW71" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ71" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="72" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>118</v>
       </c>
@@ -38972,17 +38987,17 @@
       <c r="JZ72" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KN72" s="6" t="s">
+      <c r="KO72" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU72" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX72" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="73" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW72" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ72" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>71</v>
       </c>
@@ -39365,17 +39380,17 @@
       <c r="JZ73" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KS73" s="6" t="s">
+      <c r="KT73" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU73" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX73" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="74" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW73" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ73" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="74" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>72</v>
       </c>
@@ -39739,20 +39754,20 @@
       <c r="JZ74" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK74" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KQ74" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU74" s="6" t="s">
+      <c r="KL74" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR74" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW74" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX74" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="75" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ74" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="75" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>73</v>
       </c>
@@ -40122,17 +40137,17 @@
       <c r="KB75" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KH75" s="6" t="s">
+      <c r="KI75" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU75" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX75" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="76" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW75" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ75" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="76" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>74</v>
       </c>
@@ -40507,14 +40522,20 @@
       <c r="JZ76" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU76" s="6" t="s">
+      <c r="KF76" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX76" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="77" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KV76" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW76" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ76" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="77" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>75</v>
       </c>
@@ -40906,14 +40927,14 @@
       <c r="KA77" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU77" s="6" t="s">
+      <c r="KW77" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX77" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="78" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ77" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="78" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>76</v>
       </c>
@@ -41297,17 +41318,17 @@
       <c r="KD78" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KJ78" s="6" t="s">
+      <c r="KK78" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU78" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX78" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="79" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW78" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ78" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="79" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>119</v>
       </c>
@@ -41672,14 +41693,14 @@
       <c r="JZ79" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU79" s="6" t="s">
+      <c r="KW79" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX79" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="80" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ79" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="80" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>78</v>
       </c>
@@ -42056,17 +42077,17 @@
       <c r="JZ80" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KN80" s="6" t="s">
+      <c r="KO80" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU80" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX80" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="81" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KW80" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ80" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="81" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>79</v>
       </c>
@@ -42450,14 +42471,14 @@
       <c r="JZ81" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU81" s="6" t="s">
+      <c r="KW81" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX81" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="82" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ81" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="82" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>80</v>
       </c>
@@ -42829,14 +42850,14 @@
       <c r="JZ82" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU82" s="6" t="s">
+      <c r="KW82" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX82" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="83" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ82" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="83" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>81</v>
       </c>
@@ -43210,26 +43231,26 @@
       <c r="JZ83" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK83" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KN83" s="6" t="s">
+      <c r="KL83" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KO83" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KO83" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KR83" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KU83" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX83" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="84" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KP83" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KS83" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW83" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ83" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="84" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>82</v>
       </c>
@@ -43611,14 +43632,14 @@
       <c r="JZ84" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU84" s="6" t="s">
+      <c r="KW84" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX84" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="85" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ84" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="85" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>83</v>
       </c>
@@ -43985,14 +44006,14 @@
       <c r="JZ85" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU85" s="6" t="s">
+      <c r="KW85" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX85" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="86" spans="1:310" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="KZ85" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="86" spans="1:312" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>84</v>
       </c>
@@ -44390,14 +44411,14 @@
       <c r="JZ86" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU86" s="6" t="s">
+      <c r="KW86" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX86" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="87" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ86" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="87" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>85</v>
       </c>
@@ -44767,14 +44788,14 @@
       <c r="JZ87" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU87" s="6" t="s">
+      <c r="KW87" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX87" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="88" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ87" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="88" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>2985</v>
       </c>
@@ -44808,14 +44829,14 @@
       <c r="JZ88" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU88" s="6" t="s">
+      <c r="KW88" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX88" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="89" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ88" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>1632</v>
       </c>
@@ -44844,17 +44865,17 @@
       <c r="JZ89" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KQ89" s="6" t="s">
+      <c r="KR89" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU89" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX89" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="90" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KW89" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ89" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="90" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>1633</v>
       </c>
@@ -44883,14 +44904,14 @@
       <c r="JZ90" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KU90" s="6" t="s">
+      <c r="KW90" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX90" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="91" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ90" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="91" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>1634</v>
       </c>
@@ -44927,17 +44948,17 @@
       <c r="JZ91" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KT91" s="6" t="s">
+      <c r="KU91" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KU91" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX91" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="92" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KW91" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ91" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="92" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>1641</v>
       </c>
@@ -44980,11 +45001,11 @@
       <c r="JZ92" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX92" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="93" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ92" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>1635</v>
       </c>
@@ -45022,11 +45043,11 @@
       <c r="JZ93" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX93" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="94" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ93" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="94" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>1636</v>
       </c>
@@ -45066,11 +45087,11 @@
       <c r="JZ94" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX94" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="95" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ94" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>1638</v>
       </c>
@@ -45110,11 +45131,11 @@
       <c r="JZ95" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX95" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="96" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ95" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="96" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>1639</v>
       </c>
@@ -45157,11 +45178,14 @@
       <c r="JZ96" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX96" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="97" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KU96" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KZ96" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="97" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>1637</v>
       </c>
@@ -45196,11 +45220,11 @@
       <c r="JZ97" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX97" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="98" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ97" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="98" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>1640</v>
       </c>
@@ -45238,14 +45262,14 @@
       <c r="JZ98" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KL98" s="6" t="s">
+      <c r="KM98" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX98" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="99" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ98" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="99" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>1965</v>
       </c>
@@ -45276,11 +45300,11 @@
       <c r="Z99" s="6" t="s">
         <v>1300</v>
       </c>
-      <c r="KX99" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="100" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ99" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="100" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>1684</v>
       </c>
@@ -45320,11 +45344,11 @@
       <c r="Z100" s="6" t="s">
         <v>1855</v>
       </c>
-      <c r="KX100" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="101" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ100" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="101" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>1661</v>
       </c>
@@ -45365,11 +45389,11 @@
       <c r="JZ101" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX101" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="102" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ101" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>1727</v>
       </c>
@@ -45396,11 +45420,11 @@
       <c r="Z102" s="6" t="s">
         <v>2486</v>
       </c>
-      <c r="KX102" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="103" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ102" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="103" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>1729</v>
       </c>
@@ -45429,11 +45453,11 @@
       <c r="Z103" s="6" t="s">
         <v>2486</v>
       </c>
-      <c r="KX103" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="104" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ103" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>1664</v>
       </c>
@@ -45476,11 +45500,11 @@
       <c r="JZ104" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX104" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="105" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ104" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="105" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
         <v>1666</v>
       </c>
@@ -45510,14 +45534,11 @@
       <c r="JT105" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JZ105" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX105" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="106" spans="1:310" ht="30" x14ac:dyDescent="0.25">
+      <c r="KZ105" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="106" spans="1:312" ht="30" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>1680</v>
       </c>
@@ -45557,14 +45578,23 @@
       <c r="JT106" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JZ106" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX106" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="107" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="JV106" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KP106" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KR106" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW106" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ106" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="107" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>1536</v>
       </c>
@@ -45862,20 +45892,20 @@
       <c r="JT107" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JZ107" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KB107" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KJ107" s="6" t="s">
+      <c r="KK107" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KQ107" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="108" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KR107" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KW107" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="108" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>1662</v>
       </c>
@@ -45915,17 +45945,20 @@
       <c r="JT108" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JZ108" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KB108" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX108" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="109" spans="1:310" x14ac:dyDescent="0.25">
+        <v>1535</v>
+      </c>
+      <c r="KI108" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW108" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ108" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="109" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
         <v>1723</v>
       </c>
@@ -45960,8 +45993,14 @@
       <c r="Z109" s="6" t="s">
         <v>2487</v>
       </c>
-    </row>
-    <row r="110" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KB109" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW109" s="6" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="110" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>1663</v>
       </c>
@@ -45998,14 +46037,14 @@
       <c r="JT110" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="JZ110" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KB110" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="111" spans="1:310" x14ac:dyDescent="0.25">
+        <v>1535</v>
+      </c>
+      <c r="KW110" s="6" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="111" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>1945</v>
       </c>
@@ -46043,8 +46082,17 @@
       <c r="Z111" s="6" t="s">
         <v>2487</v>
       </c>
-    </row>
-    <row r="112" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KB111" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KR111" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW111" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="112" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
         <v>2886</v>
       </c>
@@ -46071,8 +46119,17 @@
       </c>
       <c r="R112" s="45"/>
       <c r="S112" s="45"/>
-    </row>
-    <row r="113" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KB112" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KL112" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW112" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="113" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
         <v>2887</v>
       </c>
@@ -46100,7 +46157,7 @@
       <c r="R113" s="45"/>
       <c r="S113" s="45"/>
     </row>
-    <row r="114" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>1682</v>
       </c>
@@ -46135,16 +46192,19 @@
         <v>2486</v>
       </c>
       <c r="JT114" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="JZ114" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX114" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="115" spans="1:310" x14ac:dyDescent="0.25">
+        <v>1535</v>
+      </c>
+      <c r="KQ114" s="6" t="s">
+        <v>1535</v>
+      </c>
+      <c r="KW114" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ114" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="115" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
         <v>2894</v>
       </c>
@@ -46169,7 +46229,7 @@
       <c r="R115" s="45"/>
       <c r="S115" s="45"/>
     </row>
-    <row r="116" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
         <v>2895</v>
       </c>
@@ -46194,7 +46254,7 @@
       <c r="R116" s="45"/>
       <c r="S116" s="45"/>
     </row>
-    <row r="117" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>2896</v>
       </c>
@@ -46219,7 +46279,7 @@
       <c r="R117" s="45"/>
       <c r="S117" s="45"/>
     </row>
-    <row r="118" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
         <v>2897</v>
       </c>
@@ -46244,7 +46304,7 @@
       <c r="R118" s="45"/>
       <c r="S118" s="45"/>
     </row>
-    <row r="119" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
         <v>2898</v>
       </c>
@@ -46269,7 +46329,7 @@
       <c r="R119" s="45"/>
       <c r="S119" s="45"/>
     </row>
-    <row r="120" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
         <v>2899</v>
       </c>
@@ -46294,7 +46354,7 @@
       <c r="R120" s="45"/>
       <c r="S120" s="45"/>
     </row>
-    <row r="121" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
         <v>2900</v>
       </c>
@@ -46319,7 +46379,7 @@
       <c r="R121" s="45"/>
       <c r="S121" s="45"/>
     </row>
-    <row r="122" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>1668</v>
       </c>
@@ -46352,11 +46412,11 @@
       <c r="JZ122" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX122" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="123" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ122" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="123" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
         <v>1944</v>
       </c>
@@ -46383,11 +46443,11 @@
       <c r="Z123" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="KX123" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="124" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ123" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="124" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>1669</v>
       </c>
@@ -46425,11 +46485,11 @@
       <c r="JZ124" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX124" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="125" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ124" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="125" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="s">
         <v>1672</v>
       </c>
@@ -46473,11 +46533,11 @@
       <c r="JZ125" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX125" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="126" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ125" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="126" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>1670</v>
       </c>
@@ -46523,11 +46583,11 @@
       <c r="JZ126" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX126" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="127" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ126" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="127" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A127" s="6" t="s">
         <v>1628</v>
       </c>
@@ -46567,11 +46627,11 @@
       <c r="JZ127" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX127" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="128" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ127" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="128" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>1627</v>
       </c>
@@ -46609,11 +46669,11 @@
       <c r="JZ128" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX128" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="129" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ128" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="129" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>1631</v>
       </c>
@@ -46656,11 +46716,11 @@
       <c r="JZ129" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX129" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="130" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ129" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="130" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>1667</v>
       </c>
@@ -46697,11 +46757,11 @@
       <c r="JZ130" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX130" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="131" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ130" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="131" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>1537</v>
       </c>
@@ -46739,11 +46799,11 @@
       <c r="JZ131" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX131" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="132" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ131" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="132" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>1468</v>
       </c>
@@ -46787,11 +46847,11 @@
       <c r="JZ132" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX132" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="133" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ132" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="133" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>1538</v>
       </c>
@@ -46824,14 +46884,14 @@
       <c r="KE133" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KV133" s="6" t="s">
+      <c r="KX133" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KX133" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="134" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ133" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="134" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>1469</v>
       </c>
@@ -46863,11 +46923,11 @@
       <c r="JZ134" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX134" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="135" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ134" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="135" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
         <v>1471</v>
       </c>
@@ -46902,11 +46962,11 @@
       <c r="JZ135" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX135" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="136" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ135" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="136" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A136" s="15" t="s">
         <v>1539</v>
       </c>
@@ -46961,35 +47021,35 @@
       <c r="KD136" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KJ136" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KK136" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KM136" s="6" t="s">
+      <c r="KL136" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KN136" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KO136" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KP136" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KP136" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KQ136" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KV136" s="6" t="s">
+      <c r="KR136" s="6" t="s">
         <v>384</v>
       </c>
       <c r="KX136" s="6" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="137" spans="1:310" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="KZ136" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="137" spans="1:312" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
         <v>1473</v>
       </c>
@@ -47050,9 +47110,6 @@
       <c r="KD137" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KK137" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KL137" s="6" t="s">
         <v>384</v>
       </c>
@@ -47060,19 +47117,22 @@
         <v>384</v>
       </c>
       <c r="KN137" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KO137" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KP137" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="KQ137" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX137" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="138" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KR137" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ137" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="138" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A138" s="15" t="s">
         <v>1540</v>
       </c>
@@ -47109,11 +47169,11 @@
       <c r="JZ138" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX138" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="139" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ138" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="139" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A139" s="15" t="s">
         <v>1475</v>
       </c>
@@ -47148,11 +47208,11 @@
       <c r="JZ139" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX139" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="140" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ139" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="140" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
         <v>1541</v>
       </c>
@@ -47181,11 +47241,11 @@
       <c r="JZ140" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX140" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="141" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ140" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="141" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
         <v>1477</v>
       </c>
@@ -47218,11 +47278,11 @@
       <c r="JZ141" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX141" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="142" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ141" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="142" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
         <v>1478</v>
       </c>
@@ -47255,11 +47315,11 @@
       <c r="JZ142" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX142" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="143" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ142" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="143" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
         <v>1542</v>
       </c>
@@ -47289,11 +47349,11 @@
       <c r="JZ143" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX143" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="144" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ143" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="144" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
         <v>1480</v>
       </c>
@@ -47336,20 +47396,20 @@
       <c r="KB144" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KJ144" s="6" t="s">
+      <c r="KK144" s="6" t="s">
         <v>1535</v>
       </c>
-      <c r="KK144" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KM144" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="KX144" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="145" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KL144" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KN144" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="KZ144" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="145" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A145" s="15" t="s">
         <v>1543</v>
       </c>
@@ -47381,11 +47441,11 @@
       <c r="JZ145" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX145" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="146" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ145" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="146" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
         <v>1481</v>
       </c>
@@ -47420,11 +47480,11 @@
       <c r="JZ146" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX146" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="147" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ146" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="147" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
         <v>1545</v>
       </c>
@@ -47458,11 +47518,11 @@
       <c r="JZ147" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX147" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="148" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ147" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="148" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>1726</v>
       </c>
@@ -47483,11 +47543,11 @@
       <c r="Z148" s="6" t="s">
         <v>1169</v>
       </c>
-      <c r="KX148" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="149" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ148" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="149" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
         <v>1544</v>
       </c>
@@ -47523,11 +47583,11 @@
       <c r="JZ149" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX149" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="150" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ149" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="150" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
         <v>1485</v>
       </c>
@@ -47556,11 +47616,11 @@
       <c r="JZ150" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX150" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="151" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ150" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="151" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>1685</v>
       </c>
@@ -47592,11 +47652,11 @@
       <c r="Z151" s="6" t="s">
         <v>2488</v>
       </c>
-      <c r="KX151" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="152" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ151" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="152" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A152" s="15" t="s">
         <v>1546</v>
       </c>
@@ -47631,11 +47691,11 @@
       <c r="JZ152" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX152" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="153" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ152" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="153" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A153" s="15" t="s">
         <v>1487</v>
       </c>
@@ -47664,11 +47724,11 @@
       <c r="JZ153" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX153" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="154" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ153" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="154" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A154" s="15" t="s">
         <v>1489</v>
       </c>
@@ -47706,11 +47766,11 @@
       <c r="JZ154" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX154" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="155" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ154" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="155" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A155" s="15" t="s">
         <v>1488</v>
       </c>
@@ -47750,11 +47810,11 @@
       <c r="JZ155" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX155" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="156" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ155" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="156" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A156" s="15" t="s">
         <v>1490</v>
       </c>
@@ -47800,11 +47860,11 @@
       <c r="KB156" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX156" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="157" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ156" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="157" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A157" s="15" t="s">
         <v>1491</v>
       </c>
@@ -47842,11 +47902,11 @@
       <c r="JZ157" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX157" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="158" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ157" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="158" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>1731</v>
       </c>
@@ -47880,11 +47940,11 @@
       <c r="Z158" s="6" t="s">
         <v>1447</v>
       </c>
-      <c r="KX158" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="159" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ158" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="159" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
         <v>1492</v>
       </c>
@@ -47913,11 +47973,11 @@
       <c r="JZ159" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX159" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="160" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ159" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="160" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
         <v>1493</v>
       </c>
@@ -47949,11 +48009,11 @@
       <c r="JZ160" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX160" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="161" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ160" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="161" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
         <v>1734</v>
       </c>
@@ -47987,11 +48047,11 @@
       <c r="Z161" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="KX161" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="162" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ161" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="162" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
         <v>1494</v>
       </c>
@@ -48028,11 +48088,11 @@
       <c r="JZ162" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX162" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="163" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ162" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="163" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A163" s="15" t="s">
         <v>1495</v>
       </c>
@@ -48078,11 +48138,11 @@
       <c r="JZ163" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="KX163" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="164" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ163" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="164" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>1738</v>
       </c>
@@ -48116,11 +48176,11 @@
       <c r="Z164" s="6" t="s">
         <v>535</v>
       </c>
-      <c r="KX164" s="6" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="165" spans="1:310" x14ac:dyDescent="0.25">
+      <c r="KZ164" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="165" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A165" s="15" t="s">
         <v>2935</v>
       </c>
@@ -48143,7 +48203,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="166" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A166" s="15" t="s">
         <v>2943</v>
       </c>
@@ -48166,7 +48226,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="167" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A167" s="15" t="s">
         <v>2945</v>
       </c>
@@ -48189,7 +48249,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="168" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A168" s="15" t="s">
         <v>2952</v>
       </c>
@@ -48212,7 +48272,7 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="169" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A169" s="15" t="s">
         <v>2930</v>
       </c>
@@ -48235,7 +48295,7 @@
         <v>2975</v>
       </c>
     </row>
-    <row r="170" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A170" s="15" t="s">
         <v>2931</v>
       </c>
@@ -48258,7 +48318,7 @@
         <v>2976</v>
       </c>
     </row>
-    <row r="171" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A171" s="15" t="s">
         <v>2933</v>
       </c>
@@ -48281,7 +48341,7 @@
         <v>2937</v>
       </c>
     </row>
-    <row r="172" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A172" s="15" t="s">
         <v>2934</v>
       </c>
@@ -48304,7 +48364,7 @@
         <v>2934</v>
       </c>
     </row>
-    <row r="173" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A173" s="15" t="s">
         <v>2932</v>
       </c>
@@ -48327,7 +48387,7 @@
         <v>2977</v>
       </c>
     </row>
-    <row r="174" spans="1:310" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:312" x14ac:dyDescent="0.25">
       <c r="A174" s="15" t="s">
         <v>2936</v>
       </c>
@@ -48351,15 +48411,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:KX155" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:KX155">
-      <sortCondition ref="I101:I155"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:KX174">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:KZ174">
     <sortCondition ref="I171:I174"/>
   </sortState>
-  <conditionalFormatting sqref="A1:JH1 KX1:XFD1 JT1:KV1 JJ1:JR1">
+  <conditionalFormatting sqref="A1:JH1 KZ1:XFD1 JT1:KX1 JJ1:JR1">
     <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="RELATIONSHIP:">
       <formula>NOT(ISERROR(SEARCH("RELATIONSHIP:",A1)))</formula>
     </cfRule>
@@ -48376,21 +48431,21 @@
       <formula>NOT(ISERROR(SEARCH("NODE:",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="KW1">
+  <conditionalFormatting sqref="KY1">
     <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="RELATIONSHIP:">
-      <formula>NOT(ISERROR(SEARCH("RELATIONSHIP:",KW1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("RELATIONSHIP:",KY1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="TRAIT:">
-      <formula>NOT(ISERROR(SEARCH("TRAIT:",KW1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRAIT:",KY1)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"ignore"</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="STATIC:">
-      <formula>NOT(ISERROR(SEARCH("STATIC:",KW1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("STATIC:",KY1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="NODE:">
-      <formula>NOT(ISERROR(SEARCH("NODE:",KW1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NODE:",KY1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS1">
@@ -48437,10 +48492,10 @@
   <dimension ref="A1:GS1379"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="17" ySplit="10" topLeftCell="CW11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="17" ySplit="10" topLeftCell="R11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="CX11" sqref="CX11"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>